<commit_message>
feat: add parser for bar plots
</commit_message>
<xml_diff>
--- a/app/data/basisdaten_clean.xlsx
+++ b/app/data/basisdaten_clean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guadaluperomero/ProjectsTSB/innovationserhebung/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A75E88-9D03-2F45-95E9-1C7788DAAA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F57F6B-386F-F14F-BDD7-30623F7E9D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16840" firstSheet="17" activeTab="25" xr2:uid="{25BCFA3D-CBEA-9B42-8B95-A0D09F81B565}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" firstSheet="22" activeTab="29" xr2:uid="{25BCFA3D-CBEA-9B42-8B95-A0D09F81B565}"/>
   </bookViews>
   <sheets>
     <sheet name="basis_2013_ber" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,10 @@
     <sheet name="anteile_branchen_de" sheetId="26" r:id="rId24"/>
     <sheet name="relevanzbubbles_ber" sheetId="27" r:id="rId25"/>
     <sheet name="relevanzbubbles_de" sheetId="28" r:id="rId26"/>
+    <sheet name="coop_partner_2012_ber" sheetId="29" r:id="rId27"/>
+    <sheet name="coop_partner_2020_ber" sheetId="31" r:id="rId28"/>
+    <sheet name="coop_partner_2012_de" sheetId="32" r:id="rId29"/>
+    <sheet name="coop_partner_2020_de" sheetId="33" r:id="rId30"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1641" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="97">
   <si>
     <t>Nr. der Klas-
 sifikation</t>
@@ -336,6 +340,24 @@
   <si>
     <t>Umsatz mit Produktneuheiten in Mio. €</t>
   </si>
+  <si>
+    <t>insgesamt</t>
+  </si>
+  <si>
+    <t>staatl. Forschung</t>
+  </si>
+  <si>
+    <t>Kunden (privatwirtschaftl.)</t>
+  </si>
+  <si>
+    <t>Lieferanten</t>
+  </si>
+  <si>
+    <t>Wettbewerber</t>
+  </si>
+  <si>
+    <t>WZ</t>
+  </si>
 </sst>
 </file>
 
@@ -344,7 +366,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -398,6 +420,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -493,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -630,6 +665,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="8" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17372,7 +17417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB49BC20-BD07-9B4E-AF60-DA96205E68A6}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -17874,6 +17919,2655 @@
       <c r="E29" s="60">
         <v>535499</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A328FC18-3C10-8D47-B29E-409DC103D216}">
+  <dimension ref="A1:H38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="21">
+        <v>14</v>
+      </c>
+      <c r="D2" s="21">
+        <v>6</v>
+      </c>
+      <c r="E2" s="21">
+        <v>6</v>
+      </c>
+      <c r="F2" s="21">
+        <v>4</v>
+      </c>
+      <c r="G2" s="21">
+        <v>9</v>
+      </c>
+      <c r="H2" s="56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="21">
+        <v>62</v>
+      </c>
+      <c r="D3" s="21">
+        <v>50</v>
+      </c>
+      <c r="E3" s="21">
+        <v>45</v>
+      </c>
+      <c r="F3" s="21">
+        <v>28</v>
+      </c>
+      <c r="G3" s="21">
+        <v>7</v>
+      </c>
+      <c r="H3" s="56">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="21">
+        <v>0</v>
+      </c>
+      <c r="D4" s="21">
+        <v>0</v>
+      </c>
+      <c r="E4" s="21">
+        <v>0</v>
+      </c>
+      <c r="F4" s="21">
+        <v>0</v>
+      </c>
+      <c r="G4" s="21">
+        <v>0</v>
+      </c>
+      <c r="H4" s="56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="21">
+        <v>20</v>
+      </c>
+      <c r="D5" s="21">
+        <v>14</v>
+      </c>
+      <c r="E5" s="21">
+        <v>1</v>
+      </c>
+      <c r="F5" s="21">
+        <v>13</v>
+      </c>
+      <c r="G5" s="21">
+        <v>6</v>
+      </c>
+      <c r="H5" s="56">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="21">
+        <v>59</v>
+      </c>
+      <c r="D6" s="21">
+        <v>42</v>
+      </c>
+      <c r="E6" s="21">
+        <v>35</v>
+      </c>
+      <c r="F6" s="21">
+        <v>25</v>
+      </c>
+      <c r="G6" s="21">
+        <v>17</v>
+      </c>
+      <c r="H6" s="56">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="21">
+        <v>62</v>
+      </c>
+      <c r="D7" s="21">
+        <v>30</v>
+      </c>
+      <c r="E7" s="21">
+        <v>18</v>
+      </c>
+      <c r="F7" s="21">
+        <v>16</v>
+      </c>
+      <c r="G7" s="21">
+        <v>28</v>
+      </c>
+      <c r="H7" s="56">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="21">
+        <v>29</v>
+      </c>
+      <c r="D8" s="21">
+        <v>10</v>
+      </c>
+      <c r="E8" s="21">
+        <v>2</v>
+      </c>
+      <c r="F8" s="21">
+        <v>7</v>
+      </c>
+      <c r="G8" s="21">
+        <v>13</v>
+      </c>
+      <c r="H8" s="56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="21">
+        <v>20</v>
+      </c>
+      <c r="D9" s="21">
+        <v>6</v>
+      </c>
+      <c r="E9" s="21">
+        <v>5</v>
+      </c>
+      <c r="F9" s="21">
+        <v>3</v>
+      </c>
+      <c r="G9" s="21">
+        <v>6</v>
+      </c>
+      <c r="H9" s="56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="21">
+        <v>17</v>
+      </c>
+      <c r="D10" s="21">
+        <v>10</v>
+      </c>
+      <c r="E10" s="21">
+        <v>4</v>
+      </c>
+      <c r="F10" s="21">
+        <v>6</v>
+      </c>
+      <c r="G10" s="21">
+        <v>5</v>
+      </c>
+      <c r="H10" s="56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="21">
+        <v>42</v>
+      </c>
+      <c r="D11" s="21">
+        <v>27</v>
+      </c>
+      <c r="E11" s="21">
+        <v>12</v>
+      </c>
+      <c r="F11" s="21">
+        <v>5</v>
+      </c>
+      <c r="G11" s="21">
+        <v>1</v>
+      </c>
+      <c r="H11" s="56">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="21">
+        <v>18</v>
+      </c>
+      <c r="D12" s="21">
+        <v>11</v>
+      </c>
+      <c r="E12" s="21">
+        <v>7</v>
+      </c>
+      <c r="F12" s="21">
+        <v>7</v>
+      </c>
+      <c r="G12" s="21">
+        <v>13</v>
+      </c>
+      <c r="H12" s="56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="21">
+        <v>29</v>
+      </c>
+      <c r="D13" s="21">
+        <v>24</v>
+      </c>
+      <c r="E13" s="21">
+        <v>9</v>
+      </c>
+      <c r="F13" s="21">
+        <v>10</v>
+      </c>
+      <c r="G13" s="21">
+        <v>8</v>
+      </c>
+      <c r="H13" s="56">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="21">
+        <v>13</v>
+      </c>
+      <c r="D14" s="21">
+        <v>12</v>
+      </c>
+      <c r="E14" s="21">
+        <v>2</v>
+      </c>
+      <c r="F14" s="21">
+        <v>3</v>
+      </c>
+      <c r="G14" s="21">
+        <v>5</v>
+      </c>
+      <c r="H14" s="56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="21">
+        <v>82</v>
+      </c>
+      <c r="D15" s="21">
+        <v>82</v>
+      </c>
+      <c r="E15" s="21">
+        <v>55</v>
+      </c>
+      <c r="F15" s="21">
+        <v>39</v>
+      </c>
+      <c r="G15" s="21">
+        <v>0</v>
+      </c>
+      <c r="H15" s="56">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="21">
+        <v>20</v>
+      </c>
+      <c r="D16" s="21">
+        <v>10</v>
+      </c>
+      <c r="E16" s="21">
+        <v>4</v>
+      </c>
+      <c r="F16" s="21">
+        <v>5</v>
+      </c>
+      <c r="G16" s="21">
+        <v>14</v>
+      </c>
+      <c r="H16" s="56">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="19"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="56"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="21">
+        <v>36</v>
+      </c>
+      <c r="D18" s="21">
+        <v>22</v>
+      </c>
+      <c r="E18" s="21">
+        <v>15</v>
+      </c>
+      <c r="F18" s="21">
+        <v>13</v>
+      </c>
+      <c r="G18" s="21">
+        <v>12</v>
+      </c>
+      <c r="H18" s="56">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="21">
+        <v>30</v>
+      </c>
+      <c r="D19" s="21">
+        <v>22</v>
+      </c>
+      <c r="E19" s="21">
+        <v>10</v>
+      </c>
+      <c r="F19" s="21">
+        <v>7</v>
+      </c>
+      <c r="G19" s="21">
+        <v>5</v>
+      </c>
+      <c r="H19" s="56">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="19"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="56"/>
+    </row>
+    <row r="21" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A21" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="26">
+        <v>32</v>
+      </c>
+      <c r="D21" s="26">
+        <v>22</v>
+      </c>
+      <c r="E21" s="26">
+        <v>11</v>
+      </c>
+      <c r="F21" s="26">
+        <v>9</v>
+      </c>
+      <c r="G21" s="26">
+        <v>7</v>
+      </c>
+      <c r="H21" s="56">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="19"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="56"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="56"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="21">
+        <v>24</v>
+      </c>
+      <c r="D24" s="21">
+        <v>16</v>
+      </c>
+      <c r="E24" s="21">
+        <v>8</v>
+      </c>
+      <c r="F24" s="21">
+        <v>7</v>
+      </c>
+      <c r="G24" s="21">
+        <v>5</v>
+      </c>
+      <c r="H24" s="56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="21">
+        <v>33</v>
+      </c>
+      <c r="D25" s="21">
+        <v>25</v>
+      </c>
+      <c r="E25" s="21">
+        <v>12</v>
+      </c>
+      <c r="F25" s="21">
+        <v>8</v>
+      </c>
+      <c r="G25" s="21">
+        <v>6</v>
+      </c>
+      <c r="H25" s="56">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="21">
+        <v>34</v>
+      </c>
+      <c r="D26" s="21">
+        <v>21</v>
+      </c>
+      <c r="E26" s="21">
+        <v>11</v>
+      </c>
+      <c r="F26" s="21">
+        <v>8</v>
+      </c>
+      <c r="G26" s="21">
+        <v>7</v>
+      </c>
+      <c r="H26" s="56">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="21">
+        <v>42</v>
+      </c>
+      <c r="D27" s="21">
+        <v>25</v>
+      </c>
+      <c r="E27" s="21">
+        <v>14</v>
+      </c>
+      <c r="F27" s="21">
+        <v>16</v>
+      </c>
+      <c r="G27" s="21">
+        <v>17</v>
+      </c>
+      <c r="H27" s="56">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="21">
+        <v>73</v>
+      </c>
+      <c r="D28" s="21">
+        <v>66</v>
+      </c>
+      <c r="E28" s="21">
+        <v>50</v>
+      </c>
+      <c r="F28" s="21">
+        <v>45</v>
+      </c>
+      <c r="G28" s="21">
+        <v>25</v>
+      </c>
+      <c r="H28" s="56">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="21">
+        <v>75</v>
+      </c>
+      <c r="D29" s="21">
+        <v>72</v>
+      </c>
+      <c r="E29" s="21">
+        <v>61</v>
+      </c>
+      <c r="F29" s="21">
+        <v>47</v>
+      </c>
+      <c r="G29" s="21">
+        <v>18</v>
+      </c>
+      <c r="H29" s="56">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="19"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="56"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="19"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="56"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="20">
+        <v>65</v>
+      </c>
+      <c r="D32" s="21">
+        <v>49</v>
+      </c>
+      <c r="E32" s="21">
+        <v>38</v>
+      </c>
+      <c r="F32" s="21">
+        <v>23</v>
+      </c>
+      <c r="G32" s="21">
+        <v>16</v>
+      </c>
+      <c r="H32" s="56">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="20">
+        <v>39</v>
+      </c>
+      <c r="D33" s="21">
+        <v>19</v>
+      </c>
+      <c r="E33" s="21">
+        <v>15</v>
+      </c>
+      <c r="F33" s="21">
+        <v>16</v>
+      </c>
+      <c r="G33" s="21">
+        <v>15</v>
+      </c>
+      <c r="H33" s="56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="20">
+        <v>27</v>
+      </c>
+      <c r="D34" s="21">
+        <v>14</v>
+      </c>
+      <c r="E34" s="21">
+        <v>8</v>
+      </c>
+      <c r="F34" s="21">
+        <v>8</v>
+      </c>
+      <c r="G34" s="21">
+        <v>20</v>
+      </c>
+      <c r="H34" s="56">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="20">
+        <v>40</v>
+      </c>
+      <c r="D35" s="21">
+        <v>26</v>
+      </c>
+      <c r="E35" s="21">
+        <v>12</v>
+      </c>
+      <c r="F35" s="21">
+        <v>6</v>
+      </c>
+      <c r="G35" s="21">
+        <v>1</v>
+      </c>
+      <c r="H35" s="56">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="20">
+        <v>28</v>
+      </c>
+      <c r="D36" s="21">
+        <v>26</v>
+      </c>
+      <c r="E36" s="21">
+        <v>11</v>
+      </c>
+      <c r="F36" s="21">
+        <v>8</v>
+      </c>
+      <c r="G36" s="21">
+        <v>6</v>
+      </c>
+      <c r="H36" s="56">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="20">
+        <v>26</v>
+      </c>
+      <c r="D37" s="21">
+        <v>20</v>
+      </c>
+      <c r="E37" s="21">
+        <v>8</v>
+      </c>
+      <c r="F37" s="21">
+        <v>11</v>
+      </c>
+      <c r="G37" s="21">
+        <v>8</v>
+      </c>
+      <c r="H37" s="56">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="20">
+        <v>17</v>
+      </c>
+      <c r="D38" s="21">
+        <v>9</v>
+      </c>
+      <c r="E38" s="21">
+        <v>4</v>
+      </c>
+      <c r="F38" s="21">
+        <v>6</v>
+      </c>
+      <c r="G38" s="21">
+        <v>9</v>
+      </c>
+      <c r="H38" s="56">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8892AF24-D85C-4D49-A7A1-70F793B3C12F}">
+  <dimension ref="A1:H38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="56">
+        <v>7</v>
+      </c>
+      <c r="D2" s="66">
+        <v>1</v>
+      </c>
+      <c r="E2" s="66">
+        <v>1</v>
+      </c>
+      <c r="F2" s="66">
+        <v>5</v>
+      </c>
+      <c r="G2" s="66">
+        <v>5</v>
+      </c>
+      <c r="H2" s="66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="56">
+        <v>43</v>
+      </c>
+      <c r="D3" s="66">
+        <v>23</v>
+      </c>
+      <c r="E3" s="66">
+        <v>7</v>
+      </c>
+      <c r="F3" s="66">
+        <v>10</v>
+      </c>
+      <c r="G3" s="66">
+        <v>2</v>
+      </c>
+      <c r="H3" s="66">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="56">
+        <v>43</v>
+      </c>
+      <c r="D4" s="66">
+        <v>6</v>
+      </c>
+      <c r="E4" s="66">
+        <v>1</v>
+      </c>
+      <c r="F4" s="66">
+        <v>5</v>
+      </c>
+      <c r="G4" s="66">
+        <v>1</v>
+      </c>
+      <c r="H4" s="66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="56">
+        <v>8</v>
+      </c>
+      <c r="D5" s="66">
+        <v>8</v>
+      </c>
+      <c r="E5" s="66">
+        <v>1</v>
+      </c>
+      <c r="F5" s="66">
+        <v>1</v>
+      </c>
+      <c r="G5" s="66">
+        <v>0</v>
+      </c>
+      <c r="H5" s="66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="56">
+        <v>35</v>
+      </c>
+      <c r="D6" s="66">
+        <v>23</v>
+      </c>
+      <c r="E6" s="66">
+        <v>23</v>
+      </c>
+      <c r="F6" s="66">
+        <v>6</v>
+      </c>
+      <c r="G6" s="66">
+        <v>7</v>
+      </c>
+      <c r="H6" s="66">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="56">
+        <v>45</v>
+      </c>
+      <c r="D7" s="66">
+        <v>32</v>
+      </c>
+      <c r="E7" s="66">
+        <v>26</v>
+      </c>
+      <c r="F7" s="66">
+        <v>2</v>
+      </c>
+      <c r="G7" s="66">
+        <v>13</v>
+      </c>
+      <c r="H7" s="66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="56">
+        <v>38</v>
+      </c>
+      <c r="D8" s="66">
+        <v>33</v>
+      </c>
+      <c r="E8" s="66">
+        <v>1</v>
+      </c>
+      <c r="F8" s="66">
+        <v>5</v>
+      </c>
+      <c r="G8" s="66">
+        <v>0</v>
+      </c>
+      <c r="H8" s="66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="56">
+        <v>24</v>
+      </c>
+      <c r="D9" s="66">
+        <v>9</v>
+      </c>
+      <c r="E9" s="66">
+        <v>7</v>
+      </c>
+      <c r="F9" s="66">
+        <v>6</v>
+      </c>
+      <c r="G9" s="66">
+        <v>0</v>
+      </c>
+      <c r="H9" s="66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="56">
+        <v>23</v>
+      </c>
+      <c r="D10" s="66">
+        <v>1</v>
+      </c>
+      <c r="E10" s="66">
+        <v>0</v>
+      </c>
+      <c r="F10" s="66">
+        <v>0</v>
+      </c>
+      <c r="G10" s="66">
+        <v>0</v>
+      </c>
+      <c r="H10" s="66">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="56">
+        <v>34</v>
+      </c>
+      <c r="D11" s="66">
+        <v>26</v>
+      </c>
+      <c r="E11" s="66">
+        <v>10</v>
+      </c>
+      <c r="F11" s="66">
+        <v>9</v>
+      </c>
+      <c r="G11" s="66">
+        <v>7</v>
+      </c>
+      <c r="H11" s="66">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="56">
+        <v>14</v>
+      </c>
+      <c r="D12" s="66">
+        <v>2</v>
+      </c>
+      <c r="E12" s="66">
+        <v>1</v>
+      </c>
+      <c r="F12" s="66">
+        <v>6</v>
+      </c>
+      <c r="G12" s="66">
+        <v>1</v>
+      </c>
+      <c r="H12" s="66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="56">
+        <v>28</v>
+      </c>
+      <c r="D13" s="66">
+        <v>27</v>
+      </c>
+      <c r="E13" s="66">
+        <v>14</v>
+      </c>
+      <c r="F13" s="66">
+        <v>10</v>
+      </c>
+      <c r="G13" s="66">
+        <v>17</v>
+      </c>
+      <c r="H13" s="66">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="56">
+        <v>22</v>
+      </c>
+      <c r="D14" s="66">
+        <v>8</v>
+      </c>
+      <c r="E14" s="66">
+        <v>2</v>
+      </c>
+      <c r="F14" s="66">
+        <v>6</v>
+      </c>
+      <c r="G14" s="66">
+        <v>4</v>
+      </c>
+      <c r="H14" s="66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="56">
+        <v>88</v>
+      </c>
+      <c r="D15" s="66">
+        <v>75</v>
+      </c>
+      <c r="E15" s="66">
+        <v>56</v>
+      </c>
+      <c r="F15" s="66">
+        <v>35</v>
+      </c>
+      <c r="G15" s="66">
+        <v>8</v>
+      </c>
+      <c r="H15" s="66">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="56">
+        <v>20</v>
+      </c>
+      <c r="D16" s="66">
+        <v>11</v>
+      </c>
+      <c r="E16" s="66">
+        <v>3</v>
+      </c>
+      <c r="F16" s="66">
+        <v>10</v>
+      </c>
+      <c r="G16" s="66">
+        <v>5</v>
+      </c>
+      <c r="H16" s="66">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="19"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="56">
+        <v>31</v>
+      </c>
+      <c r="D18" s="66">
+        <v>19</v>
+      </c>
+      <c r="E18" s="66">
+        <v>10</v>
+      </c>
+      <c r="F18" s="66">
+        <v>5</v>
+      </c>
+      <c r="G18" s="66">
+        <v>4</v>
+      </c>
+      <c r="H18" s="66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="56">
+        <v>29</v>
+      </c>
+      <c r="D19" s="66">
+        <v>19</v>
+      </c>
+      <c r="E19" s="66">
+        <v>8</v>
+      </c>
+      <c r="F19" s="66">
+        <v>8</v>
+      </c>
+      <c r="G19" s="66">
+        <v>6</v>
+      </c>
+      <c r="H19" s="66">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="19"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="68"/>
+    </row>
+    <row r="21" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A21" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="56">
+        <v>30</v>
+      </c>
+      <c r="D21" s="70">
+        <v>19</v>
+      </c>
+      <c r="E21" s="70">
+        <v>9</v>
+      </c>
+      <c r="F21" s="70">
+        <v>8</v>
+      </c>
+      <c r="G21" s="70">
+        <v>6</v>
+      </c>
+      <c r="H21" s="70">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="19"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="68"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="56">
+        <v>19</v>
+      </c>
+      <c r="D24" s="66">
+        <v>7</v>
+      </c>
+      <c r="E24" s="66">
+        <v>4</v>
+      </c>
+      <c r="F24" s="66">
+        <v>4</v>
+      </c>
+      <c r="G24" s="66">
+        <v>2</v>
+      </c>
+      <c r="H24" s="66">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="56">
+        <v>32</v>
+      </c>
+      <c r="D25" s="66">
+        <v>25</v>
+      </c>
+      <c r="E25" s="66">
+        <v>13</v>
+      </c>
+      <c r="F25" s="66">
+        <v>11</v>
+      </c>
+      <c r="G25" s="66">
+        <v>6</v>
+      </c>
+      <c r="H25" s="66">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="56">
+        <v>30</v>
+      </c>
+      <c r="D26" s="66">
+        <v>20</v>
+      </c>
+      <c r="E26" s="66">
+        <v>10</v>
+      </c>
+      <c r="F26" s="66">
+        <v>8</v>
+      </c>
+      <c r="G26" s="66">
+        <v>8</v>
+      </c>
+      <c r="H26" s="66">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="56">
+        <v>41</v>
+      </c>
+      <c r="D27" s="66">
+        <v>29</v>
+      </c>
+      <c r="E27" s="66">
+        <v>7</v>
+      </c>
+      <c r="F27" s="66">
+        <v>7</v>
+      </c>
+      <c r="G27" s="66">
+        <v>9</v>
+      </c>
+      <c r="H27" s="66">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="56">
+        <v>71</v>
+      </c>
+      <c r="D28" s="66">
+        <v>39</v>
+      </c>
+      <c r="E28" s="66">
+        <v>17</v>
+      </c>
+      <c r="F28" s="66">
+        <v>25</v>
+      </c>
+      <c r="G28" s="66">
+        <v>15</v>
+      </c>
+      <c r="H28" s="66">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="56">
+        <v>91</v>
+      </c>
+      <c r="D29" s="66">
+        <v>59</v>
+      </c>
+      <c r="E29" s="66">
+        <v>30</v>
+      </c>
+      <c r="F29" s="66">
+        <v>25</v>
+      </c>
+      <c r="G29" s="66">
+        <v>17</v>
+      </c>
+      <c r="H29" s="66">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="19"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="68"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="68"/>
+      <c r="H30" s="68"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="19"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="68"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="68"/>
+      <c r="H31" s="68"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="56">
+        <v>61</v>
+      </c>
+      <c r="D32" s="66">
+        <v>41</v>
+      </c>
+      <c r="E32" s="66">
+        <v>33</v>
+      </c>
+      <c r="F32" s="66">
+        <v>9</v>
+      </c>
+      <c r="G32" s="66">
+        <v>10</v>
+      </c>
+      <c r="H32" s="66">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="56">
+        <v>53</v>
+      </c>
+      <c r="D33" s="66">
+        <v>42</v>
+      </c>
+      <c r="E33" s="66">
+        <v>16</v>
+      </c>
+      <c r="F33" s="66">
+        <v>5</v>
+      </c>
+      <c r="G33" s="66">
+        <v>5</v>
+      </c>
+      <c r="H33" s="66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="56">
+        <v>25</v>
+      </c>
+      <c r="D34" s="66">
+        <v>3</v>
+      </c>
+      <c r="E34" s="66">
+        <v>2</v>
+      </c>
+      <c r="F34" s="66">
+        <v>11</v>
+      </c>
+      <c r="G34" s="66">
+        <v>1</v>
+      </c>
+      <c r="H34" s="66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="56">
+        <v>33</v>
+      </c>
+      <c r="D35" s="66">
+        <v>26</v>
+      </c>
+      <c r="E35" s="66">
+        <v>10</v>
+      </c>
+      <c r="F35" s="66">
+        <v>8</v>
+      </c>
+      <c r="G35" s="66">
+        <v>7</v>
+      </c>
+      <c r="H35" s="66">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="56">
+        <v>31</v>
+      </c>
+      <c r="D36" s="66">
+        <v>19</v>
+      </c>
+      <c r="E36" s="66">
+        <v>10</v>
+      </c>
+      <c r="F36" s="66">
+        <v>11</v>
+      </c>
+      <c r="G36" s="66">
+        <v>4</v>
+      </c>
+      <c r="H36" s="66">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="56">
+        <v>28</v>
+      </c>
+      <c r="D37" s="66">
+        <v>20</v>
+      </c>
+      <c r="E37" s="66">
+        <v>9</v>
+      </c>
+      <c r="F37" s="66">
+        <v>10</v>
+      </c>
+      <c r="G37" s="66">
+        <v>15</v>
+      </c>
+      <c r="H37" s="66">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="56">
+        <v>22</v>
+      </c>
+      <c r="D38" s="66">
+        <v>2</v>
+      </c>
+      <c r="E38" s="66">
+        <v>1</v>
+      </c>
+      <c r="F38" s="66">
+        <v>1</v>
+      </c>
+      <c r="G38" s="66">
+        <v>0</v>
+      </c>
+      <c r="H38" s="66">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD8627D-4657-EE4C-962D-304C4103ABD4}">
+  <dimension ref="A1:H38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="56">
+        <v>5</v>
+      </c>
+      <c r="D2" s="21">
+        <v>4</v>
+      </c>
+      <c r="E2" s="21">
+        <v>1</v>
+      </c>
+      <c r="F2" s="21">
+        <v>4</v>
+      </c>
+      <c r="G2" s="21">
+        <v>3</v>
+      </c>
+      <c r="H2" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="56">
+        <v>36</v>
+      </c>
+      <c r="D3" s="21">
+        <v>19</v>
+      </c>
+      <c r="E3" s="21">
+        <v>12</v>
+      </c>
+      <c r="F3" s="21">
+        <v>13</v>
+      </c>
+      <c r="G3" s="21">
+        <v>16</v>
+      </c>
+      <c r="H3" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="56">
+        <v>13</v>
+      </c>
+      <c r="D4" s="21">
+        <v>4</v>
+      </c>
+      <c r="E4" s="21">
+        <v>1</v>
+      </c>
+      <c r="F4" s="21">
+        <v>8</v>
+      </c>
+      <c r="G4" s="21">
+        <v>5</v>
+      </c>
+      <c r="H4" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="56">
+        <v>20</v>
+      </c>
+      <c r="D5" s="21">
+        <v>12</v>
+      </c>
+      <c r="E5" s="21">
+        <v>5</v>
+      </c>
+      <c r="F5" s="21">
+        <v>5</v>
+      </c>
+      <c r="G5" s="21">
+        <v>7</v>
+      </c>
+      <c r="H5" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="56">
+        <v>38</v>
+      </c>
+      <c r="D6" s="21">
+        <v>22</v>
+      </c>
+      <c r="E6" s="21">
+        <v>10</v>
+      </c>
+      <c r="F6" s="21">
+        <v>12</v>
+      </c>
+      <c r="G6" s="21">
+        <v>14</v>
+      </c>
+      <c r="H6" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="56">
+        <v>32</v>
+      </c>
+      <c r="D7" s="21">
+        <v>18</v>
+      </c>
+      <c r="E7" s="21">
+        <v>8</v>
+      </c>
+      <c r="F7" s="21">
+        <v>14</v>
+      </c>
+      <c r="G7" s="21">
+        <v>17</v>
+      </c>
+      <c r="H7" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="56">
+        <v>20</v>
+      </c>
+      <c r="D8" s="21">
+        <v>10</v>
+      </c>
+      <c r="E8" s="21">
+        <v>6</v>
+      </c>
+      <c r="F8" s="21">
+        <v>8</v>
+      </c>
+      <c r="G8" s="21">
+        <v>5</v>
+      </c>
+      <c r="H8" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="56">
+        <v>17</v>
+      </c>
+      <c r="D9" s="21">
+        <v>11</v>
+      </c>
+      <c r="E9" s="21">
+        <v>6</v>
+      </c>
+      <c r="F9" s="21">
+        <v>6</v>
+      </c>
+      <c r="G9" s="21">
+        <v>11</v>
+      </c>
+      <c r="H9" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="56">
+        <v>13</v>
+      </c>
+      <c r="D10" s="21">
+        <v>8</v>
+      </c>
+      <c r="E10" s="21">
+        <v>7</v>
+      </c>
+      <c r="F10" s="21">
+        <v>3</v>
+      </c>
+      <c r="G10" s="21">
+        <v>3</v>
+      </c>
+      <c r="H10" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="56">
+        <v>29</v>
+      </c>
+      <c r="D11" s="21">
+        <v>21</v>
+      </c>
+      <c r="E11" s="21">
+        <v>10</v>
+      </c>
+      <c r="F11" s="21">
+        <v>11</v>
+      </c>
+      <c r="G11" s="21">
+        <v>7</v>
+      </c>
+      <c r="H11" s="21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="56">
+        <v>15</v>
+      </c>
+      <c r="D12" s="21">
+        <v>3</v>
+      </c>
+      <c r="E12" s="21">
+        <v>1</v>
+      </c>
+      <c r="F12" s="21">
+        <v>4</v>
+      </c>
+      <c r="G12" s="21">
+        <v>4</v>
+      </c>
+      <c r="H12" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="56">
+        <v>27</v>
+      </c>
+      <c r="D13" s="21">
+        <v>18</v>
+      </c>
+      <c r="E13" s="21">
+        <v>4</v>
+      </c>
+      <c r="F13" s="21">
+        <v>15</v>
+      </c>
+      <c r="G13" s="21">
+        <v>17</v>
+      </c>
+      <c r="H13" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="56">
+        <v>23</v>
+      </c>
+      <c r="D14" s="21">
+        <v>17</v>
+      </c>
+      <c r="E14" s="21">
+        <v>9</v>
+      </c>
+      <c r="F14" s="21">
+        <v>11</v>
+      </c>
+      <c r="G14" s="21">
+        <v>10</v>
+      </c>
+      <c r="H14" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="56">
+        <v>86</v>
+      </c>
+      <c r="D15" s="21">
+        <v>75</v>
+      </c>
+      <c r="E15" s="21">
+        <v>55</v>
+      </c>
+      <c r="F15" s="21">
+        <v>50</v>
+      </c>
+      <c r="G15" s="21">
+        <v>32</v>
+      </c>
+      <c r="H15" s="21">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="56">
+        <v>20</v>
+      </c>
+      <c r="D16" s="21">
+        <v>3</v>
+      </c>
+      <c r="E16" s="21">
+        <v>2</v>
+      </c>
+      <c r="F16" s="21">
+        <v>6</v>
+      </c>
+      <c r="G16" s="21">
+        <v>9</v>
+      </c>
+      <c r="H16" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="19"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="56">
+        <v>24</v>
+      </c>
+      <c r="D18" s="21">
+        <v>14</v>
+      </c>
+      <c r="E18" s="21">
+        <v>7</v>
+      </c>
+      <c r="F18" s="21">
+        <v>9</v>
+      </c>
+      <c r="G18" s="21">
+        <v>11</v>
+      </c>
+      <c r="H18" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="56">
+        <v>26</v>
+      </c>
+      <c r="D19" s="21">
+        <v>17</v>
+      </c>
+      <c r="E19" s="21">
+        <v>9</v>
+      </c>
+      <c r="F19" s="21">
+        <v>11</v>
+      </c>
+      <c r="G19" s="21">
+        <v>9</v>
+      </c>
+      <c r="H19" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="19"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A21" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="56">
+        <v>25</v>
+      </c>
+      <c r="D21" s="26">
+        <v>15</v>
+      </c>
+      <c r="E21" s="26">
+        <v>7</v>
+      </c>
+      <c r="F21" s="26">
+        <v>10</v>
+      </c>
+      <c r="G21" s="26">
+        <v>10</v>
+      </c>
+      <c r="H21" s="26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="19"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="56">
+        <v>19</v>
+      </c>
+      <c r="D24" s="21">
+        <v>10</v>
+      </c>
+      <c r="E24" s="21">
+        <v>6</v>
+      </c>
+      <c r="F24" s="21">
+        <v>8</v>
+      </c>
+      <c r="G24" s="21">
+        <v>8</v>
+      </c>
+      <c r="H24" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="56">
+        <v>20</v>
+      </c>
+      <c r="D25" s="21">
+        <v>13</v>
+      </c>
+      <c r="E25" s="21">
+        <v>6</v>
+      </c>
+      <c r="F25" s="21">
+        <v>8</v>
+      </c>
+      <c r="G25" s="21">
+        <v>8</v>
+      </c>
+      <c r="H25" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="56">
+        <v>24</v>
+      </c>
+      <c r="D26" s="21">
+        <v>14</v>
+      </c>
+      <c r="E26" s="21">
+        <v>7</v>
+      </c>
+      <c r="F26" s="21">
+        <v>8</v>
+      </c>
+      <c r="G26" s="21">
+        <v>8</v>
+      </c>
+      <c r="H26" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="56">
+        <v>34</v>
+      </c>
+      <c r="D27" s="21">
+        <v>21</v>
+      </c>
+      <c r="E27" s="21">
+        <v>9</v>
+      </c>
+      <c r="F27" s="21">
+        <v>11</v>
+      </c>
+      <c r="G27" s="21">
+        <v>14</v>
+      </c>
+      <c r="H27" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="56">
+        <v>51</v>
+      </c>
+      <c r="D28" s="21">
+        <v>36</v>
+      </c>
+      <c r="E28" s="21">
+        <v>16</v>
+      </c>
+      <c r="F28" s="21">
+        <v>24</v>
+      </c>
+      <c r="G28" s="21">
+        <v>24</v>
+      </c>
+      <c r="H28" s="21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="56">
+        <v>84</v>
+      </c>
+      <c r="D29" s="21">
+        <v>71</v>
+      </c>
+      <c r="E29" s="21">
+        <v>46</v>
+      </c>
+      <c r="F29" s="21">
+        <v>55</v>
+      </c>
+      <c r="G29" s="21">
+        <v>58</v>
+      </c>
+      <c r="H29" s="21">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="19"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="19"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="56"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="56"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="56"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56"/>
+      <c r="G37" s="56"/>
+      <c r="H37" s="56"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="56"/>
+      <c r="H38" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19056,6 +21750,833 @@
       <c r="I40" s="21"/>
       <c r="J40" s="21"/>
       <c r="K40" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7FE29F2-626E-664E-9813-62F674DA7A6D}">
+  <dimension ref="A1:H38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="67">
+        <v>8</v>
+      </c>
+      <c r="D2" s="66">
+        <v>4</v>
+      </c>
+      <c r="E2" s="66">
+        <v>2</v>
+      </c>
+      <c r="F2" s="66">
+        <v>5</v>
+      </c>
+      <c r="G2" s="66">
+        <v>6</v>
+      </c>
+      <c r="H2" s="66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="67">
+        <v>35</v>
+      </c>
+      <c r="D3" s="66">
+        <v>21</v>
+      </c>
+      <c r="E3" s="66">
+        <v>9</v>
+      </c>
+      <c r="F3" s="66">
+        <v>11</v>
+      </c>
+      <c r="G3" s="66">
+        <v>10</v>
+      </c>
+      <c r="H3" s="66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="67">
+        <v>10</v>
+      </c>
+      <c r="D4" s="66">
+        <v>2</v>
+      </c>
+      <c r="E4" s="66">
+        <v>1</v>
+      </c>
+      <c r="F4" s="66">
+        <v>4</v>
+      </c>
+      <c r="G4" s="66">
+        <v>4</v>
+      </c>
+      <c r="H4" s="66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="67">
+        <v>17</v>
+      </c>
+      <c r="D5" s="66">
+        <v>12</v>
+      </c>
+      <c r="E5" s="66">
+        <v>5</v>
+      </c>
+      <c r="F5" s="66">
+        <v>4</v>
+      </c>
+      <c r="G5" s="66">
+        <v>7</v>
+      </c>
+      <c r="H5" s="66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="67">
+        <v>43</v>
+      </c>
+      <c r="D6" s="66">
+        <v>26</v>
+      </c>
+      <c r="E6" s="66">
+        <v>15</v>
+      </c>
+      <c r="F6" s="66">
+        <v>13</v>
+      </c>
+      <c r="G6" s="66">
+        <v>11</v>
+      </c>
+      <c r="H6" s="66">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="67">
+        <v>33</v>
+      </c>
+      <c r="D7" s="66">
+        <v>23</v>
+      </c>
+      <c r="E7" s="66">
+        <v>8</v>
+      </c>
+      <c r="F7" s="66">
+        <v>9</v>
+      </c>
+      <c r="G7" s="66">
+        <v>10</v>
+      </c>
+      <c r="H7" s="66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="67">
+        <v>11</v>
+      </c>
+      <c r="D8" s="66">
+        <v>7</v>
+      </c>
+      <c r="E8" s="66">
+        <v>2</v>
+      </c>
+      <c r="F8" s="66">
+        <v>1</v>
+      </c>
+      <c r="G8" s="66">
+        <v>3</v>
+      </c>
+      <c r="H8" s="66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="67">
+        <v>17</v>
+      </c>
+      <c r="D9" s="66">
+        <v>9</v>
+      </c>
+      <c r="E9" s="66">
+        <v>4</v>
+      </c>
+      <c r="F9" s="66">
+        <v>4</v>
+      </c>
+      <c r="G9" s="66">
+        <v>8</v>
+      </c>
+      <c r="H9" s="66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="67">
+        <v>21</v>
+      </c>
+      <c r="D10" s="66">
+        <v>7</v>
+      </c>
+      <c r="E10" s="66">
+        <v>1</v>
+      </c>
+      <c r="F10" s="66">
+        <v>5</v>
+      </c>
+      <c r="G10" s="66">
+        <v>6</v>
+      </c>
+      <c r="H10" s="66">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="67">
+        <v>29</v>
+      </c>
+      <c r="D11" s="66">
+        <v>19</v>
+      </c>
+      <c r="E11" s="66">
+        <v>7</v>
+      </c>
+      <c r="F11" s="66">
+        <v>8</v>
+      </c>
+      <c r="G11" s="66">
+        <v>5</v>
+      </c>
+      <c r="H11" s="66">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="67">
+        <v>22</v>
+      </c>
+      <c r="D12" s="66">
+        <v>3</v>
+      </c>
+      <c r="E12" s="66">
+        <v>0</v>
+      </c>
+      <c r="F12" s="66">
+        <v>4</v>
+      </c>
+      <c r="G12" s="66">
+        <v>8</v>
+      </c>
+      <c r="H12" s="66">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="67">
+        <v>31</v>
+      </c>
+      <c r="D13" s="66">
+        <v>19</v>
+      </c>
+      <c r="E13" s="66">
+        <v>5</v>
+      </c>
+      <c r="F13" s="66">
+        <v>23</v>
+      </c>
+      <c r="G13" s="66">
+        <v>5</v>
+      </c>
+      <c r="H13" s="66">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="67">
+        <v>15</v>
+      </c>
+      <c r="D14" s="66">
+        <v>12</v>
+      </c>
+      <c r="E14" s="66">
+        <v>5</v>
+      </c>
+      <c r="F14" s="66">
+        <v>8</v>
+      </c>
+      <c r="G14" s="66">
+        <v>2</v>
+      </c>
+      <c r="H14" s="66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="67">
+        <v>82</v>
+      </c>
+      <c r="D15" s="66">
+        <v>67</v>
+      </c>
+      <c r="E15" s="66">
+        <v>35</v>
+      </c>
+      <c r="F15" s="66">
+        <v>41</v>
+      </c>
+      <c r="G15" s="66">
+        <v>20</v>
+      </c>
+      <c r="H15" s="66">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="67">
+        <v>13</v>
+      </c>
+      <c r="D16" s="66">
+        <v>7</v>
+      </c>
+      <c r="E16" s="66">
+        <v>1</v>
+      </c>
+      <c r="F16" s="66">
+        <v>6</v>
+      </c>
+      <c r="G16" s="66">
+        <v>5</v>
+      </c>
+      <c r="H16" s="66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="19"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="67">
+        <v>23</v>
+      </c>
+      <c r="D18" s="66">
+        <v>14</v>
+      </c>
+      <c r="E18" s="66">
+        <v>6</v>
+      </c>
+      <c r="F18" s="66">
+        <v>7</v>
+      </c>
+      <c r="G18" s="66">
+        <v>8</v>
+      </c>
+      <c r="H18" s="66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="67">
+        <v>24</v>
+      </c>
+      <c r="D19" s="66">
+        <v>15</v>
+      </c>
+      <c r="E19" s="66">
+        <v>5</v>
+      </c>
+      <c r="F19" s="66">
+        <v>9</v>
+      </c>
+      <c r="G19" s="66">
+        <v>5</v>
+      </c>
+      <c r="H19" s="66">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="19"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="68"/>
+    </row>
+    <row r="21" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A21" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="71">
+        <v>24</v>
+      </c>
+      <c r="D21" s="70">
+        <v>15</v>
+      </c>
+      <c r="E21" s="70">
+        <v>6</v>
+      </c>
+      <c r="F21" s="70">
+        <v>8</v>
+      </c>
+      <c r="G21" s="70">
+        <v>7</v>
+      </c>
+      <c r="H21" s="70">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="19"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="68"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="67">
+        <v>16</v>
+      </c>
+      <c r="D24" s="66">
+        <v>10</v>
+      </c>
+      <c r="E24" s="66">
+        <v>2</v>
+      </c>
+      <c r="F24" s="66">
+        <v>8</v>
+      </c>
+      <c r="G24" s="66">
+        <v>3</v>
+      </c>
+      <c r="H24" s="66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="67">
+        <v>19</v>
+      </c>
+      <c r="D25" s="66">
+        <v>12</v>
+      </c>
+      <c r="E25" s="66">
+        <v>6</v>
+      </c>
+      <c r="F25" s="66">
+        <v>4</v>
+      </c>
+      <c r="G25" s="66">
+        <v>5</v>
+      </c>
+      <c r="H25" s="66">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="67">
+        <v>25</v>
+      </c>
+      <c r="D26" s="66">
+        <v>15</v>
+      </c>
+      <c r="E26" s="66">
+        <v>6</v>
+      </c>
+      <c r="F26" s="66">
+        <v>9</v>
+      </c>
+      <c r="G26" s="66">
+        <v>7</v>
+      </c>
+      <c r="H26" s="66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="67">
+        <v>30</v>
+      </c>
+      <c r="D27" s="66">
+        <v>20</v>
+      </c>
+      <c r="E27" s="66">
+        <v>7</v>
+      </c>
+      <c r="F27" s="66">
+        <v>8</v>
+      </c>
+      <c r="G27" s="66">
+        <v>8</v>
+      </c>
+      <c r="H27" s="66">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="67">
+        <v>50</v>
+      </c>
+      <c r="D28" s="66">
+        <v>35</v>
+      </c>
+      <c r="E28" s="66">
+        <v>14</v>
+      </c>
+      <c r="F28" s="66">
+        <v>15</v>
+      </c>
+      <c r="G28" s="66">
+        <v>22</v>
+      </c>
+      <c r="H28" s="66">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="67">
+        <v>85</v>
+      </c>
+      <c r="D29" s="66">
+        <v>63</v>
+      </c>
+      <c r="E29" s="66">
+        <v>31</v>
+      </c>
+      <c r="F29" s="66">
+        <v>30</v>
+      </c>
+      <c r="G29" s="66">
+        <v>45</v>
+      </c>
+      <c r="H29" s="66">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="19"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="19"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="56"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="56"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="56"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56"/>
+      <c r="G37" s="56"/>
+      <c r="H37" s="56"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="56"/>
+      <c r="H38" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: use real data for the base line plot
</commit_message>
<xml_diff>
--- a/app/data/basisdaten_clean.xlsx
+++ b/app/data/basisdaten_clean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guadaluperomero/ProjectsTSB/innovationserhebung/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F57F6B-386F-F14F-BDD7-30623F7E9D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FC83D8-7C2A-AF4E-9BB2-A4CBF371A309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" firstSheet="22" activeTab="29" xr2:uid="{25BCFA3D-CBEA-9B42-8B95-A0D09F81B565}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="2" xr2:uid="{25BCFA3D-CBEA-9B42-8B95-A0D09F81B565}"/>
   </bookViews>
   <sheets>
     <sheet name="basis_2013_ber" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="96">
   <si>
     <t>Nr. der Klas-
 sifikation</t>
@@ -282,9 +282,6 @@
   </si>
   <si>
     <t>Anzahl Beschäf-tigte*</t>
-  </si>
-  <si>
-    <t>v</t>
   </si>
   <si>
     <t>Jahr</t>
@@ -16218,22 +16215,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="C1" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="D1" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="E1" t="s">
         <v>76</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="56" t="s">
         <v>77</v>
-      </c>
-      <c r="F1" s="56" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -16403,22 +16400,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="C1" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="D1" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="E1" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="F1" t="s">
         <v>77</v>
-      </c>
-      <c r="F1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -16582,7 +16579,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1">
         <v>2012</v>
@@ -16647,7 +16644,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="57">
         <f>100-SUM(B3:B5)</f>
@@ -16675,7 +16672,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1">
         <v>2012</v>
@@ -16730,7 +16727,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="57">
         <f t="shared" ref="B6" si="0">100-SUM(B2:B5)</f>
@@ -16769,13 +16766,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="62" t="s">
-        <v>82</v>
-      </c>
       <c r="E1" s="62" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -17035,7 +17032,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" s="56">
         <v>0</v>
@@ -17086,7 +17083,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" s="56">
         <v>0</v>
@@ -17120,7 +17117,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B22" s="56">
         <v>0</v>
@@ -17157,7 +17154,7 @@
         <v>45</v>
       </c>
       <c r="B24" s="56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" s="61">
         <v>105</v>
@@ -17174,7 +17171,7 @@
         <v>47</v>
       </c>
       <c r="B25" s="56" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C25" s="61">
         <v>125</v>
@@ -17191,7 +17188,7 @@
         <v>48</v>
       </c>
       <c r="B26" s="56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C26" s="61">
         <v>375</v>
@@ -17208,7 +17205,7 @@
         <v>49</v>
       </c>
       <c r="B27" s="56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C27" s="61">
         <v>413</v>
@@ -17225,7 +17222,7 @@
         <v>50</v>
       </c>
       <c r="B28" s="56" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C28" s="61">
         <v>437</v>
@@ -17242,7 +17239,7 @@
         <v>51</v>
       </c>
       <c r="B29" s="56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C29" s="61">
         <v>1587</v>
@@ -17256,7 +17253,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30" s="56">
         <v>0</v>
@@ -17435,13 +17432,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="64" t="s">
-        <v>82</v>
-      </c>
       <c r="E1" s="64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -17701,7 +17698,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -17752,7 +17749,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -17786,7 +17783,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -17823,7 +17820,7 @@
         <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" s="60">
         <v>1427</v>
@@ -17840,7 +17837,7 @@
         <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C25" s="60">
         <v>1929</v>
@@ -17857,7 +17854,7 @@
         <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C26" s="60">
         <v>3615</v>
@@ -17874,7 +17871,7 @@
         <v>49</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C27" s="60">
         <v>11351</v>
@@ -17891,7 +17888,7 @@
         <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C28" s="60">
         <v>16210</v>
@@ -17908,7 +17905,7 @@
         <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C29" s="60">
         <v>72490</v>
@@ -17937,28 +17934,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="56" t="s">
+      <c r="F1" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="G1" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="56" t="s">
+      <c r="H1" s="56" t="s">
         <v>94</v>
-      </c>
-      <c r="H1" s="56" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -18848,28 +18845,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="56" t="s">
+      <c r="F1" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="G1" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="56" t="s">
+      <c r="H1" s="56" t="s">
         <v>94</v>
-      </c>
-      <c r="H1" s="56" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -19759,28 +19756,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="56" t="s">
+      <c r="F1" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="G1" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="56" t="s">
+      <c r="H1" s="56" t="s">
         <v>94</v>
-      </c>
-      <c r="H1" s="56" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -20578,7 +20575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3617C5-31E3-BA4A-AE6E-FA8E9080AA63}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -20742,8 +20739,8 @@
       <c r="C6" s="20">
         <v>334</v>
       </c>
-      <c r="D6" s="21" t="s">
-        <v>72</v>
+      <c r="D6" s="21">
+        <v>139</v>
       </c>
       <c r="E6" s="21">
         <v>113</v>
@@ -21760,7 +21757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7FE29F2-626E-664E-9813-62F674DA7A6D}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -21768,28 +21765,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="56" t="s">
+      <c r="F1" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="G1" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="56" t="s">
+      <c r="H1" s="56" t="s">
         <v>94</v>
-      </c>
-      <c r="H1" s="56" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feature: add import and plot for cooperation according to region data
</commit_message>
<xml_diff>
--- a/app/data/basisdaten_clean.xlsx
+++ b/app/data/basisdaten_clean.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guadaluperomero/ProjectsTSB/innovationserhebung/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FC83D8-7C2A-AF4E-9BB2-A4CBF371A309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129FF03C-EDE2-8446-A100-62A0D43C997A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="2" xr2:uid="{25BCFA3D-CBEA-9B42-8B95-A0D09F81B565}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" firstSheet="26" activeTab="30" xr2:uid="{25BCFA3D-CBEA-9B42-8B95-A0D09F81B565}"/>
   </bookViews>
   <sheets>
     <sheet name="basis_2013_ber" sheetId="1" r:id="rId1"/>
@@ -43,6 +43,10 @@
     <sheet name="coop_partner_2020_ber" sheetId="31" r:id="rId28"/>
     <sheet name="coop_partner_2012_de" sheetId="32" r:id="rId29"/>
     <sheet name="coop_partner_2020_de" sheetId="33" r:id="rId30"/>
+    <sheet name="coop_region_2012_ber" sheetId="34" r:id="rId31"/>
+    <sheet name="coop_region_2012_de" sheetId="35" r:id="rId32"/>
+    <sheet name="coop_region_2020_ber" sheetId="36" r:id="rId33"/>
+    <sheet name="coop_region_2020_de" sheetId="37" r:id="rId34"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2216" uniqueCount="102">
   <si>
     <t>Nr. der Klas-
 sifikation</t>
@@ -355,6 +359,24 @@
   <si>
     <t>WZ</t>
   </si>
+  <si>
+    <t>der Region</t>
+  </si>
+  <si>
+    <t>anderen Regionen in Deutschland</t>
+  </si>
+  <si>
+    <t>anderen europäischen Ländern</t>
+  </si>
+  <si>
+    <t>den USA</t>
+  </si>
+  <si>
+    <t>Asien</t>
+  </si>
+  <si>
+    <t>anderen Ländern</t>
+  </si>
 </sst>
 </file>
 
@@ -525,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -671,6 +693,12 @@
     </xf>
     <xf numFmtId="1" fontId="9" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -17927,7 +17955,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20575,7 +20603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3617C5-31E3-BA4A-AE6E-FA8E9080AA63}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -22574,6 +22602,3324 @@
       <c r="F38" s="56"/>
       <c r="G38" s="56"/>
       <c r="H38" s="56"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F37096C-7559-CA40-8E34-33BBEFF02349}">
+  <dimension ref="A1:H39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1" s="56" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="73" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="73" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" s="73" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="56"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="21">
+        <v>14</v>
+      </c>
+      <c r="D3" s="21">
+        <v>6</v>
+      </c>
+      <c r="E3" s="21">
+        <v>6</v>
+      </c>
+      <c r="F3" s="21">
+        <v>4</v>
+      </c>
+      <c r="G3" s="21">
+        <v>3</v>
+      </c>
+      <c r="H3" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="21">
+        <v>59</v>
+      </c>
+      <c r="D4" s="21">
+        <v>45</v>
+      </c>
+      <c r="E4" s="21">
+        <v>41</v>
+      </c>
+      <c r="F4" s="21">
+        <v>11</v>
+      </c>
+      <c r="G4" s="21">
+        <v>10</v>
+      </c>
+      <c r="H4" s="21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="21">
+        <v>0</v>
+      </c>
+      <c r="D5" s="21">
+        <v>0</v>
+      </c>
+      <c r="E5" s="21">
+        <v>0</v>
+      </c>
+      <c r="F5" s="21">
+        <v>0</v>
+      </c>
+      <c r="G5" s="21">
+        <v>0</v>
+      </c>
+      <c r="H5" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="21">
+        <v>14</v>
+      </c>
+      <c r="D6" s="21">
+        <v>8</v>
+      </c>
+      <c r="E6" s="21">
+        <v>1</v>
+      </c>
+      <c r="F6" s="21">
+        <v>0</v>
+      </c>
+      <c r="G6" s="21">
+        <v>0</v>
+      </c>
+      <c r="H6" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="21">
+        <v>45</v>
+      </c>
+      <c r="D7" s="21">
+        <v>42</v>
+      </c>
+      <c r="E7" s="21">
+        <v>20</v>
+      </c>
+      <c r="F7" s="21">
+        <v>8</v>
+      </c>
+      <c r="G7" s="21">
+        <v>8</v>
+      </c>
+      <c r="H7" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="21">
+        <v>44</v>
+      </c>
+      <c r="D8" s="21">
+        <v>25</v>
+      </c>
+      <c r="E8" s="21">
+        <v>20</v>
+      </c>
+      <c r="F8" s="21">
+        <v>3</v>
+      </c>
+      <c r="G8" s="21">
+        <v>3</v>
+      </c>
+      <c r="H8" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="21">
+        <v>10</v>
+      </c>
+      <c r="D9" s="21">
+        <v>29</v>
+      </c>
+      <c r="E9" s="21">
+        <v>2</v>
+      </c>
+      <c r="F9" s="21">
+        <v>0</v>
+      </c>
+      <c r="G9" s="21">
+        <v>0</v>
+      </c>
+      <c r="H9" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="21">
+        <v>20</v>
+      </c>
+      <c r="D10" s="21">
+        <v>14</v>
+      </c>
+      <c r="E10" s="21">
+        <v>5</v>
+      </c>
+      <c r="F10" s="21">
+        <v>1</v>
+      </c>
+      <c r="G10" s="21">
+        <v>1</v>
+      </c>
+      <c r="H10" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="21">
+        <v>10</v>
+      </c>
+      <c r="D11" s="21">
+        <v>11</v>
+      </c>
+      <c r="E11" s="21">
+        <v>7</v>
+      </c>
+      <c r="F11" s="21">
+        <v>0</v>
+      </c>
+      <c r="G11" s="21">
+        <v>4</v>
+      </c>
+      <c r="H11" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="21">
+        <v>20</v>
+      </c>
+      <c r="D12" s="21">
+        <v>28</v>
+      </c>
+      <c r="E12" s="21">
+        <v>8</v>
+      </c>
+      <c r="F12" s="21">
+        <v>0</v>
+      </c>
+      <c r="G12" s="21">
+        <v>0</v>
+      </c>
+      <c r="H12" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="21">
+        <v>18</v>
+      </c>
+      <c r="D13" s="21">
+        <v>11</v>
+      </c>
+      <c r="E13" s="21">
+        <v>11</v>
+      </c>
+      <c r="F13" s="21">
+        <v>0</v>
+      </c>
+      <c r="G13" s="21">
+        <v>0</v>
+      </c>
+      <c r="H13" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="21">
+        <v>22</v>
+      </c>
+      <c r="D14" s="21">
+        <v>23</v>
+      </c>
+      <c r="E14" s="21">
+        <v>17</v>
+      </c>
+      <c r="F14" s="21">
+        <v>0</v>
+      </c>
+      <c r="G14" s="21">
+        <v>0</v>
+      </c>
+      <c r="H14" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="21">
+        <v>11</v>
+      </c>
+      <c r="D15" s="21">
+        <v>9</v>
+      </c>
+      <c r="E15" s="21">
+        <v>2</v>
+      </c>
+      <c r="F15" s="21">
+        <v>0</v>
+      </c>
+      <c r="G15" s="21">
+        <v>0</v>
+      </c>
+      <c r="H15" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="21">
+        <v>66</v>
+      </c>
+      <c r="D16" s="21">
+        <v>62</v>
+      </c>
+      <c r="E16" s="21">
+        <v>35</v>
+      </c>
+      <c r="F16" s="21">
+        <v>14</v>
+      </c>
+      <c r="G16" s="21">
+        <v>0</v>
+      </c>
+      <c r="H16" s="21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="21">
+        <v>18</v>
+      </c>
+      <c r="D17" s="21">
+        <v>14</v>
+      </c>
+      <c r="E17" s="21">
+        <v>3</v>
+      </c>
+      <c r="F17" s="21">
+        <v>0</v>
+      </c>
+      <c r="G17" s="21">
+        <v>0</v>
+      </c>
+      <c r="H17" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="19"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="21">
+        <v>27</v>
+      </c>
+      <c r="D19" s="21">
+        <v>23</v>
+      </c>
+      <c r="E19" s="21">
+        <v>12</v>
+      </c>
+      <c r="F19" s="21">
+        <v>3</v>
+      </c>
+      <c r="G19" s="21">
+        <v>3</v>
+      </c>
+      <c r="H19" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="21">
+        <v>19</v>
+      </c>
+      <c r="D20" s="21">
+        <v>20</v>
+      </c>
+      <c r="E20" s="21">
+        <v>9</v>
+      </c>
+      <c r="F20" s="21">
+        <v>1</v>
+      </c>
+      <c r="G20" s="21">
+        <v>0</v>
+      </c>
+      <c r="H20" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="19"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+    </row>
+    <row r="22" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A22" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="26">
+        <v>22</v>
+      </c>
+      <c r="D22" s="26">
+        <v>21</v>
+      </c>
+      <c r="E22" s="26">
+        <v>10</v>
+      </c>
+      <c r="F22" s="26">
+        <v>2</v>
+      </c>
+      <c r="G22" s="26">
+        <v>1</v>
+      </c>
+      <c r="H22" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="19"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="19"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="21">
+        <v>16</v>
+      </c>
+      <c r="D25" s="21">
+        <v>15</v>
+      </c>
+      <c r="E25" s="21">
+        <v>4</v>
+      </c>
+      <c r="F25" s="21">
+        <v>0</v>
+      </c>
+      <c r="G25" s="21">
+        <v>1</v>
+      </c>
+      <c r="H25" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="21">
+        <v>20</v>
+      </c>
+      <c r="D26" s="21">
+        <v>22</v>
+      </c>
+      <c r="E26" s="21">
+        <v>11</v>
+      </c>
+      <c r="F26" s="21">
+        <v>2</v>
+      </c>
+      <c r="G26" s="21">
+        <v>0</v>
+      </c>
+      <c r="H26" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="21">
+        <v>25</v>
+      </c>
+      <c r="D27" s="21">
+        <v>22</v>
+      </c>
+      <c r="E27" s="21">
+        <v>11</v>
+      </c>
+      <c r="F27" s="21">
+        <v>1</v>
+      </c>
+      <c r="G27" s="21">
+        <v>0</v>
+      </c>
+      <c r="H27" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="21">
+        <v>30</v>
+      </c>
+      <c r="D28" s="21">
+        <v>29</v>
+      </c>
+      <c r="E28" s="21">
+        <v>12</v>
+      </c>
+      <c r="F28" s="21">
+        <v>2</v>
+      </c>
+      <c r="G28" s="21">
+        <v>2</v>
+      </c>
+      <c r="H28" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="21">
+        <v>73</v>
+      </c>
+      <c r="D29" s="21">
+        <v>63</v>
+      </c>
+      <c r="E29" s="21">
+        <v>54</v>
+      </c>
+      <c r="F29" s="21">
+        <v>25</v>
+      </c>
+      <c r="G29" s="21">
+        <v>24</v>
+      </c>
+      <c r="H29" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="21">
+        <v>70</v>
+      </c>
+      <c r="D30" s="21">
+        <v>74</v>
+      </c>
+      <c r="E30" s="21">
+        <v>66</v>
+      </c>
+      <c r="F30" s="21">
+        <v>34</v>
+      </c>
+      <c r="G30" s="21">
+        <v>31</v>
+      </c>
+      <c r="H30" s="21">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="19"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="19"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="21">
+        <v>48</v>
+      </c>
+      <c r="D33" s="21">
+        <v>50</v>
+      </c>
+      <c r="E33" s="21">
+        <v>21</v>
+      </c>
+      <c r="F33" s="21">
+        <v>4</v>
+      </c>
+      <c r="G33" s="21">
+        <v>4</v>
+      </c>
+      <c r="H33" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="21">
+        <v>27</v>
+      </c>
+      <c r="D34" s="21">
+        <v>24</v>
+      </c>
+      <c r="E34" s="21">
+        <v>12</v>
+      </c>
+      <c r="F34" s="21">
+        <v>5</v>
+      </c>
+      <c r="G34" s="21">
+        <v>5</v>
+      </c>
+      <c r="H34" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="21">
+        <v>27</v>
+      </c>
+      <c r="D35" s="21">
+        <v>14</v>
+      </c>
+      <c r="E35" s="21">
+        <v>14</v>
+      </c>
+      <c r="F35" s="21">
+        <v>0</v>
+      </c>
+      <c r="G35" s="21">
+        <v>0</v>
+      </c>
+      <c r="H35" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="21">
+        <v>20</v>
+      </c>
+      <c r="D36" s="21">
+        <v>26</v>
+      </c>
+      <c r="E36" s="21">
+        <v>8</v>
+      </c>
+      <c r="F36" s="21">
+        <v>0</v>
+      </c>
+      <c r="G36" s="21">
+        <v>0</v>
+      </c>
+      <c r="H36" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="21">
+        <v>23</v>
+      </c>
+      <c r="D37" s="21">
+        <v>21</v>
+      </c>
+      <c r="E37" s="21">
+        <v>8</v>
+      </c>
+      <c r="F37" s="21">
+        <v>3</v>
+      </c>
+      <c r="G37" s="21">
+        <v>0</v>
+      </c>
+      <c r="H37" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="21">
+        <v>18</v>
+      </c>
+      <c r="D38" s="21">
+        <v>19</v>
+      </c>
+      <c r="E38" s="21">
+        <v>13</v>
+      </c>
+      <c r="F38" s="21">
+        <v>0</v>
+      </c>
+      <c r="G38" s="21">
+        <v>0</v>
+      </c>
+      <c r="H38" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="21">
+        <v>11</v>
+      </c>
+      <c r="D39" s="21">
+        <v>12</v>
+      </c>
+      <c r="E39" s="21">
+        <v>6</v>
+      </c>
+      <c r="F39" s="21">
+        <v>1</v>
+      </c>
+      <c r="G39" s="21">
+        <v>3</v>
+      </c>
+      <c r="H39" s="21">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B88AB3-21CC-DA43-8C02-907780E2EA1D}">
+  <dimension ref="A1:H39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="72" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="72" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="72" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="72" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" s="72" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>21</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>41</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>23</v>
+      </c>
+      <c r="D7">
+        <v>23</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <v>21</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>37</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>22</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14">
+        <v>18</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>9</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15">
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16">
+        <v>59</v>
+      </c>
+      <c r="D16">
+        <v>60</v>
+      </c>
+      <c r="E16">
+        <v>52</v>
+      </c>
+      <c r="F16">
+        <v>25</v>
+      </c>
+      <c r="G16">
+        <v>25</v>
+      </c>
+      <c r="H16">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17">
+        <v>14</v>
+      </c>
+      <c r="D17">
+        <v>12</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19">
+        <v>22</v>
+      </c>
+      <c r="D19">
+        <v>11</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A22" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22">
+        <v>17</v>
+      </c>
+      <c r="D22">
+        <v>17</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25">
+        <v>11</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26">
+        <v>16</v>
+      </c>
+      <c r="D26">
+        <v>21</v>
+      </c>
+      <c r="E26">
+        <v>7</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27">
+        <v>18</v>
+      </c>
+      <c r="D27">
+        <v>16</v>
+      </c>
+      <c r="E27">
+        <v>6</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28">
+        <v>25</v>
+      </c>
+      <c r="D28">
+        <v>22</v>
+      </c>
+      <c r="E28">
+        <v>17</v>
+      </c>
+      <c r="F28">
+        <v>4</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29">
+        <v>36</v>
+      </c>
+      <c r="D29">
+        <v>46</v>
+      </c>
+      <c r="E29">
+        <v>16</v>
+      </c>
+      <c r="F29">
+        <v>4</v>
+      </c>
+      <c r="G29">
+        <v>4</v>
+      </c>
+      <c r="H29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30">
+        <v>63</v>
+      </c>
+      <c r="D30">
+        <v>48</v>
+      </c>
+      <c r="E30">
+        <v>26</v>
+      </c>
+      <c r="F30">
+        <v>10</v>
+      </c>
+      <c r="G30">
+        <v>13</v>
+      </c>
+      <c r="H30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="6"/>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33">
+        <v>26</v>
+      </c>
+      <c r="D33">
+        <v>41</v>
+      </c>
+      <c r="E33">
+        <v>6</v>
+      </c>
+      <c r="F33">
+        <v>4</v>
+      </c>
+      <c r="G33">
+        <v>10</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34">
+        <v>48</v>
+      </c>
+      <c r="D34">
+        <v>11</v>
+      </c>
+      <c r="E34">
+        <v>4</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>3</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35">
+        <v>13</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <v>12</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36">
+        <v>14</v>
+      </c>
+      <c r="D36">
+        <v>21</v>
+      </c>
+      <c r="E36">
+        <v>6</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37">
+        <v>21</v>
+      </c>
+      <c r="D37">
+        <v>19</v>
+      </c>
+      <c r="E37">
+        <v>11</v>
+      </c>
+      <c r="F37">
+        <v>4</v>
+      </c>
+      <c r="G37">
+        <v>5</v>
+      </c>
+      <c r="H37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38">
+        <v>22</v>
+      </c>
+      <c r="D38">
+        <v>17</v>
+      </c>
+      <c r="E38">
+        <v>10</v>
+      </c>
+      <c r="F38">
+        <v>5</v>
+      </c>
+      <c r="G38">
+        <v>5</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>21</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4127A38E-1EC4-954D-9DB2-9DE0917309B4}">
+  <dimension ref="A1:H39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="72" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="72" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="72" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="72" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" s="72" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="8">
+        <v>4</v>
+      </c>
+      <c r="D3" s="8">
+        <v>5</v>
+      </c>
+      <c r="E3" s="8">
+        <v>4</v>
+      </c>
+      <c r="F3" s="8">
+        <v>2</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="8">
+        <v>24</v>
+      </c>
+      <c r="D4" s="8">
+        <v>25</v>
+      </c>
+      <c r="E4" s="8">
+        <v>14</v>
+      </c>
+      <c r="F4" s="8">
+        <v>4</v>
+      </c>
+      <c r="G4" s="8">
+        <v>3</v>
+      </c>
+      <c r="H4" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8">
+        <v>10</v>
+      </c>
+      <c r="D5" s="8">
+        <v>4</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="8">
+        <v>13</v>
+      </c>
+      <c r="D6" s="8">
+        <v>12</v>
+      </c>
+      <c r="E6" s="8">
+        <v>4</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="8">
+        <v>27</v>
+      </c>
+      <c r="D7" s="8">
+        <v>25</v>
+      </c>
+      <c r="E7" s="8">
+        <v>11</v>
+      </c>
+      <c r="F7" s="8">
+        <v>5</v>
+      </c>
+      <c r="G7" s="8">
+        <v>3</v>
+      </c>
+      <c r="H7" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="8">
+        <v>21</v>
+      </c>
+      <c r="D8" s="8">
+        <v>25</v>
+      </c>
+      <c r="E8" s="8">
+        <v>10</v>
+      </c>
+      <c r="F8" s="8">
+        <v>2</v>
+      </c>
+      <c r="G8" s="8">
+        <v>2</v>
+      </c>
+      <c r="H8" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="8">
+        <v>11</v>
+      </c>
+      <c r="D9" s="8">
+        <v>15</v>
+      </c>
+      <c r="E9" s="8">
+        <v>3</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0</v>
+      </c>
+      <c r="H9" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="8">
+        <v>14</v>
+      </c>
+      <c r="D10" s="8">
+        <v>13</v>
+      </c>
+      <c r="E10" s="8">
+        <v>5</v>
+      </c>
+      <c r="F10" s="8">
+        <v>3</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+      <c r="H10" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="8">
+        <v>11</v>
+      </c>
+      <c r="D11" s="8">
+        <v>4</v>
+      </c>
+      <c r="E11" s="8">
+        <v>1</v>
+      </c>
+      <c r="F11" s="8">
+        <v>1</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="8">
+        <v>19</v>
+      </c>
+      <c r="D12" s="8">
+        <v>20</v>
+      </c>
+      <c r="E12" s="8">
+        <v>5</v>
+      </c>
+      <c r="F12" s="8">
+        <v>1</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1</v>
+      </c>
+      <c r="H12" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="8">
+        <v>11</v>
+      </c>
+      <c r="D13" s="8">
+        <v>12</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0</v>
+      </c>
+      <c r="H13" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="8">
+        <v>16</v>
+      </c>
+      <c r="D14" s="8">
+        <v>24</v>
+      </c>
+      <c r="E14" s="8">
+        <v>7</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0</v>
+      </c>
+      <c r="H14" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="8">
+        <v>17</v>
+      </c>
+      <c r="D15" s="8">
+        <v>14</v>
+      </c>
+      <c r="E15" s="8">
+        <v>4</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+      <c r="H15" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="8">
+        <v>56</v>
+      </c>
+      <c r="D16" s="8">
+        <v>66</v>
+      </c>
+      <c r="E16" s="8">
+        <v>42</v>
+      </c>
+      <c r="F16" s="8">
+        <v>10</v>
+      </c>
+      <c r="G16" s="8">
+        <v>4</v>
+      </c>
+      <c r="H16" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="8">
+        <v>12</v>
+      </c>
+      <c r="D17" s="8">
+        <v>13</v>
+      </c>
+      <c r="E17" s="8">
+        <v>10</v>
+      </c>
+      <c r="F17" s="8">
+        <v>1</v>
+      </c>
+      <c r="G17" s="8">
+        <v>1</v>
+      </c>
+      <c r="H17" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="8">
+        <v>16</v>
+      </c>
+      <c r="D19" s="8">
+        <v>16</v>
+      </c>
+      <c r="E19" s="8">
+        <v>7</v>
+      </c>
+      <c r="F19" s="8">
+        <v>2</v>
+      </c>
+      <c r="G19" s="8">
+        <v>1</v>
+      </c>
+      <c r="H19" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="8">
+        <v>18</v>
+      </c>
+      <c r="D20" s="8">
+        <v>18</v>
+      </c>
+      <c r="E20" s="8">
+        <v>6</v>
+      </c>
+      <c r="F20" s="8">
+        <v>1</v>
+      </c>
+      <c r="G20" s="8">
+        <v>1</v>
+      </c>
+      <c r="H20" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A22" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="11">
+        <v>17</v>
+      </c>
+      <c r="D22" s="11">
+        <v>17</v>
+      </c>
+      <c r="E22" s="11">
+        <v>7</v>
+      </c>
+      <c r="F22" s="11">
+        <v>2</v>
+      </c>
+      <c r="G22" s="11">
+        <v>1</v>
+      </c>
+      <c r="H22" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="8">
+        <v>13</v>
+      </c>
+      <c r="D25" s="8">
+        <v>13</v>
+      </c>
+      <c r="E25" s="8">
+        <v>4</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0</v>
+      </c>
+      <c r="H25" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="8">
+        <v>14</v>
+      </c>
+      <c r="D26" s="8">
+        <v>12</v>
+      </c>
+      <c r="E26" s="8">
+        <v>5</v>
+      </c>
+      <c r="F26" s="8">
+        <v>1</v>
+      </c>
+      <c r="G26" s="8">
+        <v>1</v>
+      </c>
+      <c r="H26" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="8">
+        <v>17</v>
+      </c>
+      <c r="D27" s="8">
+        <v>16</v>
+      </c>
+      <c r="E27" s="8">
+        <v>6</v>
+      </c>
+      <c r="F27" s="8">
+        <v>1</v>
+      </c>
+      <c r="G27" s="8">
+        <v>0</v>
+      </c>
+      <c r="H27" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="8">
+        <v>20</v>
+      </c>
+      <c r="D28" s="8">
+        <v>25</v>
+      </c>
+      <c r="E28" s="8">
+        <v>8</v>
+      </c>
+      <c r="F28" s="8">
+        <v>3</v>
+      </c>
+      <c r="G28" s="8">
+        <v>2</v>
+      </c>
+      <c r="H28" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="8">
+        <v>32</v>
+      </c>
+      <c r="D29" s="8">
+        <v>42</v>
+      </c>
+      <c r="E29" s="8">
+        <v>24</v>
+      </c>
+      <c r="F29" s="8">
+        <v>11</v>
+      </c>
+      <c r="G29" s="8">
+        <v>8</v>
+      </c>
+      <c r="H29" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="8">
+        <v>73</v>
+      </c>
+      <c r="D30" s="8">
+        <v>80</v>
+      </c>
+      <c r="E30" s="8">
+        <v>60</v>
+      </c>
+      <c r="F30" s="8">
+        <v>39</v>
+      </c>
+      <c r="G30" s="8">
+        <v>30</v>
+      </c>
+      <c r="H30" s="8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="6"/>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807574F5-FF77-854A-A93F-8E1CF13D6163}">
+  <dimension ref="A1:H39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="72" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="72" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="72" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="72" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" s="72" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>23</v>
+      </c>
+      <c r="D7">
+        <v>31</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12">
+        <v>21</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <v>17</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14">
+        <v>21</v>
+      </c>
+      <c r="D14">
+        <v>24</v>
+      </c>
+      <c r="E14">
+        <v>14</v>
+      </c>
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16">
+        <v>56</v>
+      </c>
+      <c r="D16">
+        <v>59</v>
+      </c>
+      <c r="E16">
+        <v>36</v>
+      </c>
+      <c r="F16">
+        <v>24</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>13</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>16</v>
+      </c>
+      <c r="E20">
+        <v>6</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+      <c r="A22" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22">
+        <v>15</v>
+      </c>
+      <c r="D22">
+        <v>15</v>
+      </c>
+      <c r="E22">
+        <v>6</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26">
+        <v>12</v>
+      </c>
+      <c r="D26">
+        <v>12</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27">
+        <v>19</v>
+      </c>
+      <c r="D27">
+        <v>15</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28">
+        <v>19</v>
+      </c>
+      <c r="D28">
+        <v>21</v>
+      </c>
+      <c r="E28">
+        <v>10</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29">
+        <v>30</v>
+      </c>
+      <c r="D29">
+        <v>39</v>
+      </c>
+      <c r="E29">
+        <v>21</v>
+      </c>
+      <c r="F29">
+        <v>10</v>
+      </c>
+      <c r="G29">
+        <v>9</v>
+      </c>
+      <c r="H29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30">
+        <v>59</v>
+      </c>
+      <c r="D30">
+        <v>67</v>
+      </c>
+      <c r="E30">
+        <v>40</v>
+      </c>
+      <c r="F30">
+        <v>26</v>
+      </c>
+      <c r="G30">
+        <v>23</v>
+      </c>
+      <c r="H30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="6"/>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: First IP data is from 2012 and not 2014
</commit_message>
<xml_diff>
--- a/app/data/basisdaten_clean.xlsx
+++ b/app/data/basisdaten_clean.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guadaluperomero/ProjectsTSB/innovationserhebung/app/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthieu/dev/innovationserhebung/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94787883-4D56-3248-A476-7060BF50CAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04D967B-125A-194B-8A71-60505476AAFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15260" yWindow="-28300" windowWidth="24940" windowHeight="26560" firstSheet="36" activeTab="41" xr2:uid="{25BCFA3D-CBEA-9B42-8B95-A0D09F81B565}"/>
+    <workbookView xWindow="15260" yWindow="-28300" windowWidth="24940" windowHeight="26560" firstSheet="32" activeTab="34" xr2:uid="{25BCFA3D-CBEA-9B42-8B95-A0D09F81B565}"/>
   </bookViews>
   <sheets>
     <sheet name="basis_2013_ber" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,9 @@
     <sheet name="coop_region_2012_de" sheetId="35" r:id="rId32"/>
     <sheet name="coop_region_2020_ber" sheetId="36" r:id="rId33"/>
     <sheet name="coop_region_2020_de" sheetId="37" r:id="rId34"/>
-    <sheet name="protection_2012_ber" sheetId="42" r:id="rId35"/>
+    <sheet name="protection_2014_ber" sheetId="42" r:id="rId35"/>
     <sheet name="protection_2020_ber" sheetId="43" r:id="rId36"/>
-    <sheet name="protection_2012_de" sheetId="40" r:id="rId37"/>
+    <sheet name="protection_2014_de" sheetId="40" r:id="rId37"/>
     <sheet name="protection_2020_de" sheetId="41" r:id="rId38"/>
     <sheet name="public_funding_2012_ber" sheetId="44" r:id="rId39"/>
     <sheet name="public_funding_2020_ber" sheetId="45" r:id="rId40"/>
@@ -775,7 +775,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
     <dxf>
@@ -920,9 +920,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -960,7 +960,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1066,7 +1066,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1208,7 +1208,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -26003,8 +26003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B9D5ED-1821-684A-BE84-B774B2FEECBB}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27409,8 +27409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C2E48A-BB55-9949-AE02-B813B2BB5A43}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView zoomScale="132" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31700,7 +31700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8059DFE-4CC2-FA43-9912-3A775AA99AFE}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>

</xml_diff>